<commit_message>
CIDC-1108 add 5 new optional columns to PBMC manifest for TCRseq; bump for schemas #495
</commit_message>
<xml_diff>
--- a/tests/models/templates/examples/broken/pbmc_manifest.bad_date.xlsx
+++ b/tests/models/templates/examples/broken/pbmc_manifest.bad_date.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" state="visible" r:id="rId2"/>
@@ -699,6 +699,76 @@
       <text>
         <r>
           <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The type of derivative or analyte extracted from the specimen to be shipped for testing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Volume of the analyte or derivative shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Volume units of each analyte or derivative shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The concentration of analyte or derivative shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The concentration units for the analyte or derivative shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="0">
+      <text>
+        <r>
+          <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
@@ -709,7 +779,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="0">
+    <comment ref="Y4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -723,7 +793,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U4" authorId="0">
+    <comment ref="Z4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V4" authorId="0">
+    <comment ref="AA4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -751,7 +821,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W4" authorId="0">
+    <comment ref="AB4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -765,7 +835,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X4" authorId="0">
+    <comment ref="AC4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -779,7 +849,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y4" authorId="0">
+    <comment ref="AD4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -793,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z4" authorId="0">
+    <comment ref="AE4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -807,7 +877,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA4" authorId="0">
+    <comment ref="AF4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -821,7 +891,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB4" authorId="0">
+    <comment ref="AG4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -840,7 +910,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6634" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6657" uniqueCount="345">
   <si>
     <t xml:space="preserve">LEGEND</t>
   </si>
@@ -1793,6 +1863,21 @@
     <t xml:space="preserve">Processed sample concentration units</t>
   </si>
   <si>
+    <t xml:space="preserve">Processed sample derivative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample derivative volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample derivative volume units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample derivative concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample derivative concentration units</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pbmc viability</t>
   </si>
   <si>
@@ -1835,6 +1920,12 @@
     <t xml:space="preserve">Plasma</t>
   </si>
   <si>
+    <t xml:space="preserve">Tumor DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microliters</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
@@ -1864,7 +1955,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1892,6 +1983,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -2126,7 +2224,7 @@
       <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
@@ -2800,7 +2898,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.66"/>
   </cols>
@@ -3385,11 +3483,11 @@
   </sheetPr>
   <dimension ref="A1:C2018"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.66"/>
   </cols>
@@ -13593,7 +13691,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -24010,15 +24108,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB2004"/>
+  <dimension ref="A1:AG2004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="1" style="0" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="1" style="0" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="19" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="24" style="0" width="30.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24055,18 +24155,23 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="2" t="s">
-        <v>303</v>
-      </c>
+      <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="X3" s="2" t="s">
+        <v>303</v>
+      </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -24153,6 +24258,21 @@
       <c r="AB4" s="4" t="s">
         <v>326</v>
       </c>
+      <c r="AC4" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -24165,16 +24285,16 @@
         <v>276</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>272</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>273</v>
@@ -24195,7 +24315,7 @@
         <v>192</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O5" s="0" t="n">
         <v>1</v>
@@ -24209,35 +24329,50 @@
       <c r="R5" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S5" s="0" t="n">
-        <v>1</v>
+      <c r="S5" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="9" t="s">
-        <v>131</v>
+        <v>0</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>337</v>
       </c>
       <c r="V5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W5" s="0" t="n">
+      <c r="W5" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AE5" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AF5" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="AB5" s="0" t="s">
-        <v>331</v>
+      <c r="AG5" s="0" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24251,16 +24386,16 @@
         <v>286</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>272</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>283</v>
@@ -24281,7 +24416,7 @@
         <v>192</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O6" s="0" t="n">
         <v>2</v>
@@ -24295,31 +24430,46 @@
       <c r="R6" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S6" s="0" t="n">
-        <v>1</v>
+      <c r="S6" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U6" s="9" t="s">
-        <v>151</v>
+        <v>0</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>337</v>
       </c>
       <c r="V6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W6" s="0" t="n">
+      <c r="W6" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="AD6" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AE6" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AA6" s="9" t="s">
+      <c r="AF6" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -24334,16 +24484,16 @@
         <v>276</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>272</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>287</v>
@@ -24364,7 +24514,7 @@
         <v>192</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O7" s="0" t="n">
         <v>3</v>
@@ -24378,31 +24528,46 @@
       <c r="R7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S7" s="0" t="n">
-        <v>1</v>
+      <c r="S7" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="T7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U7" s="9" t="s">
-        <v>161</v>
+        <v>0</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>337</v>
       </c>
       <c r="V7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W7" s="0" t="n">
+      <c r="W7" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="X7" s="9" t="s">
+      <c r="AC7" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="AD7" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="Z7" s="9" t="s">
+      <c r="AE7" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AA7" s="9" t="s">
+      <c r="AF7" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -24417,16 +24582,16 @@
         <v>276</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>290</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>291</v>
@@ -24447,7 +24612,7 @@
         <v>192</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O8" s="0" t="n">
         <v>4</v>
@@ -24461,31 +24626,46 @@
       <c r="R8" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S8" s="0" t="n">
-        <v>1</v>
+      <c r="S8" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>178</v>
+        <v>0</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>337</v>
       </c>
       <c r="V8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W8" s="0" t="n">
+      <c r="W8" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="AC8" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="Y8" s="9" t="s">
+      <c r="AD8" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="Z8" s="9" t="s">
+      <c r="AE8" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AA8" s="9" t="s">
+      <c r="AF8" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -24500,16 +24680,16 @@
         <v>286</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>290</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>294</v>
@@ -24530,7 +24710,7 @@
         <v>192</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O9" s="0" t="n">
         <v>5</v>
@@ -24544,31 +24724,46 @@
       <c r="R9" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S9" s="0" t="n">
-        <v>1</v>
+      <c r="S9" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U9" s="9" t="s">
-        <v>178</v>
+        <v>0</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>337</v>
       </c>
       <c r="V9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W9" s="0" t="n">
+      <c r="W9" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="X9" s="9" t="s">
+      <c r="AC9" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="Y9" s="9" t="s">
+      <c r="AD9" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="Z9" s="9" t="s">
+      <c r="AE9" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AA9" s="9" t="s">
+      <c r="AF9" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -24583,16 +24778,16 @@
         <v>276</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>290</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>297</v>
@@ -24613,7 +24808,7 @@
         <v>192</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="O10" s="0" t="n">
         <v>6</v>
@@ -24627,31 +24822,46 @@
       <c r="R10" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="S10" s="0" t="n">
-        <v>1</v>
+      <c r="S10" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U10" s="9" t="s">
-        <v>178</v>
+        <v>0</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>337</v>
       </c>
       <c r="V10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W10" s="0" t="n">
+      <c r="W10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="X10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="X10" s="9" t="s">
+      <c r="AC10" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="Y10" s="9" t="s">
+      <c r="AD10" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="Z10" s="9" t="s">
+      <c r="AE10" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AA10" s="9" t="s">
+      <c r="AF10" s="9" t="s">
         <v>135</v>
       </c>
     </row>
@@ -34630,26 +34840,26 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="I3:R3"/>
-    <mergeCell ref="S3:AB3"/>
+    <mergeCell ref="X3:AG3"/>
   </mergeCells>
-  <dataValidations count="24">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA5:AA10" type="list">
+  <dataValidations count="27">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AF5:AF10" type="list">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Z5:Z10" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE5:AE10" type="list">
       <formula1>"Replacement Not Requested,Replacement Requested,Replacement Tested,Not Reported,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y5:Y10" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD5:AD10" type="list">
       <formula1>"Pass,Fail,Not Reported,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X5:X10" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC5:AC10" type="list">
       <formula1>"RT,4oC,(-20)oC,(-80)oC,LN,Not Reported,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U5:U10" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Z5:Z10" type="list">
       <formula1>"Yes,No,Not Reported,Other"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -34709,24 +34919,36 @@
       <formula1>'Data Dictionary'!$P$2:$P$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U11:U2004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Z11:Z2004" type="list">
       <formula1>'Data Dictionary'!$Q$2:$Q$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="X11:X2004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC11:AC2004" type="list">
       <formula1>'Data Dictionary'!$R$2:$R$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Y11:Y2004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD11:AD2004" type="list">
       <formula1>'Data Dictionary'!$S$2:$S$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="Z11:Z2004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE11:AE2004" type="list">
       <formula1>'Data Dictionary'!$T$2:$T$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA11:AA2004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AF11:AF2004" type="list">
       <formula1>'Data Dictionary'!$U$2:$U$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="S11:S2004" type="list">
+      <formula1>'Data Dictionary'!$M$2:$M$7</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U11:U2004" type="list">
+      <formula1>'Data Dictionary'!$N$2:$N$5</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W11:W2004" type="list">
+      <formula1>'Data Dictionary'!$O$2:$O$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>